<commit_message>
adicionado a função de atualizar os itens
</commit_message>
<xml_diff>
--- a/bancodedados/lucasGuedes.xlsx
+++ b/bancodedados/lucasGuedes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,15 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Questões</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -449,12 +454,15 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -464,12 +472,15 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
+      <c r="B3" t="n">
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> E</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -479,12 +490,15 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B4" t="n">
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -494,12 +508,15 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
+      <c r="B5" t="n">
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> E</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -509,12 +526,15 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+      <c r="B6" t="n">
+        <v>4</v>
       </c>
       <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> D</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -524,12 +544,15 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B7" t="n">
+        <v>5</v>
       </c>
       <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -539,12 +562,15 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="B8" t="n">
+        <v>6</v>
       </c>
       <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -554,12 +580,15 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
+      <c r="B9" t="n">
+        <v>7</v>
       </c>
       <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> D</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -569,12 +598,15 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B10" t="n">
+        <v>8</v>
       </c>
       <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -584,12 +616,15 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B11" t="n">
+        <v>9</v>
       </c>
       <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -599,12 +634,15 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B12" t="n">
+        <v>10</v>
       </c>
       <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -614,12 +652,15 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B13" t="n">
+        <v>11</v>
       </c>
       <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -629,12 +670,15 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B14" t="n">
+        <v>12</v>
       </c>
       <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -644,12 +688,15 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B15" t="n">
+        <v>13</v>
       </c>
       <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -659,12 +706,15 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B16" t="n">
+        <v>14</v>
       </c>
       <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -674,12 +724,15 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B17" t="n">
+        <v>15</v>
       </c>
       <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> C</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -689,12 +742,15 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+      <c r="B18" t="n">
+        <v>16</v>
       </c>
       <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> B</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -704,12 +760,15 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="B19" t="n">
+        <v>17</v>
       </c>
       <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -719,12 +778,15 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+      <c r="B20" t="n">
+        <v>18</v>
       </c>
       <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> B</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -734,12 +796,15 @@
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+      <c r="B21" t="n">
+        <v>19</v>
       </c>
       <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> B</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -749,12 +814,15 @@
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -764,12 +832,15 @@
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -779,12 +850,15 @@
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -794,12 +868,15 @@
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" t="n">
+        <v>23</v>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -809,12 +886,15 @@
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -824,12 +904,15 @@
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="B27" t="n">
+        <v>25</v>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -839,12 +922,15 @@
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -854,12 +940,15 @@
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B29" t="n">
+        <v>27</v>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -869,12 +958,15 @@
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="B30" t="n">
+        <v>28</v>
+      </c>
+      <c r="C30" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -884,12 +976,15 @@
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B31" t="n">
+        <v>29</v>
+      </c>
+      <c r="C31" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -899,12 +994,15 @@
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -914,12 +1012,15 @@
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" t="n">
+        <v>31</v>
+      </c>
+      <c r="C33" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -929,12 +1030,15 @@
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" t="n">
+        <v>32</v>
+      </c>
+      <c r="C34" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -944,12 +1048,15 @@
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B35" t="n">
+        <v>33</v>
+      </c>
+      <c r="C35" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -959,12 +1066,15 @@
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B36" t="n">
+        <v>34</v>
+      </c>
+      <c r="C36" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -974,12 +1084,15 @@
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" t="n">
+        <v>35</v>
+      </c>
+      <c r="C37" t="inlineStr">
         <is>
           <t>C</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -989,12 +1102,15 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" t="n">
+        <v>36</v>
+      </c>
+      <c r="C38" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -1004,12 +1120,15 @@
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" t="n">
+        <v>37</v>
+      </c>
+      <c r="C39" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -1019,12 +1138,15 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B40" t="n">
+        <v>38</v>
+      </c>
+      <c r="C40" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>
@@ -1034,12 +1156,15 @@
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" t="n">
+        <v>39</v>
+      </c>
+      <c r="C41" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Peso</t>
         </is>

</xml_diff>